<commit_message>
Add except for HTTP and JSON
</commit_message>
<xml_diff>
--- a/weather_data.xlsx
+++ b/weather_data.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -458,262 +458,262 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>6.1</v>
+        <v>5.9</v>
       </c>
       <c r="B2" t="n">
-        <v>5.8</v>
+        <v>6</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Ю</t>
+          <t>ЮЗ</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>992.8</v>
+        <v>994.9</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Дождь - 0.4
-Ливень - 0.0
-Снег - 0.07</t>
+          <t>Дождь - 0.0
+Ливень - 0.0
+Снег - 0.0</t>
         </is>
       </c>
       <c r="F2" s="1" t="n">
-        <v>45580.6997428851</v>
+        <v>45580.99404122325</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>6.1</v>
+        <v>5.9</v>
       </c>
       <c r="B3" t="n">
-        <v>5.8</v>
+        <v>6</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Ю</t>
+          <t>ЮЗ</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>992.8</v>
+        <v>994.9</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Дождь - 0.4
-Ливень - 0.0
-Снег - 0.07</t>
+          <t>Дождь - 0.0
+Ливень - 0.0
+Снег - 0.0</t>
         </is>
       </c>
       <c r="F3" s="1" t="n">
-        <v>45580.69962711774</v>
+        <v>45580.99402684862</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>6.1</v>
+        <v>5.9</v>
       </c>
       <c r="B4" t="n">
-        <v>5.8</v>
+        <v>6</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Ю</t>
+          <t>ЮЗ</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>992.8</v>
+        <v>994.9</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Дождь - 0.4
+          <t>Дождь - 0.8
 Ливень - 0.0
 Снег - 0.07</t>
         </is>
       </c>
       <c r="F4" s="1" t="n">
-        <v>45580.69951134113</v>
+        <v>45580.99402511361</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>6.1</v>
+        <v>5.9</v>
       </c>
       <c r="B5" t="n">
-        <v>5.8</v>
+        <v>6</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Ю</t>
+          <t>ЮЗ</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>992.8</v>
+        <v>994.9</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Дождь - 0.4
-Ливень - 0.0
-Снег - 0.07</t>
+          <t>Дождь - 0.0
+Ливень - 0.0
+Снег - 0.0</t>
         </is>
       </c>
       <c r="F5" s="1" t="n">
-        <v>45580.69939683618</v>
+        <v>45580.99401505614</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>6.1</v>
+        <v>5.9</v>
       </c>
       <c r="B6" t="n">
-        <v>5.8</v>
+        <v>6</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Ю</t>
+          <t>ЮЗ</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>992.8</v>
+        <v>994.9</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Дождь - 0.4
-Ливень - 0.0
-Снег - 0.07</t>
+          <t>Дождь - 0.0
+Ливень - 0.0
+Снег - 0.0</t>
         </is>
       </c>
       <c r="F6" s="1" t="n">
-        <v>45580.69928435126</v>
+        <v>45580.99400483284</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6.1</v>
+        <v>5.9</v>
       </c>
       <c r="B7" t="n">
-        <v>5.8</v>
+        <v>6</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Ю</t>
+          <t>ЮЗ</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>992.8</v>
+        <v>994.9</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Дождь - 0.4
-Ливень - 0.0
-Снег - 0.07</t>
+          <t>Дождь - 0.0
+Ливень - 0.0
+Снег - 0.0</t>
         </is>
       </c>
       <c r="F7" s="1" t="n">
-        <v>45580.6991669813</v>
+        <v>45580.99399292153</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6.1</v>
+        <v>5.9</v>
       </c>
       <c r="B8" t="n">
-        <v>5.8</v>
+        <v>6</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Ю</t>
+          <t>ЮЗ</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>992.8</v>
+        <v>994.9</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Дождь - 0.4
-Ливень - 0.0
-Снег - 0.07</t>
+          <t>Дождь - 0.0
+Ливень - 0.0
+Снег - 0.0</t>
         </is>
       </c>
       <c r="F8" s="1" t="n">
-        <v>45580.69905208873</v>
+        <v>45580.99398033474</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>6.1</v>
+        <v>5.9</v>
       </c>
       <c r="B9" t="n">
-        <v>5.8</v>
+        <v>6</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Ю</t>
+          <t>ЮЗ</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>992.8</v>
+        <v>994.9</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Дождь - 0.4
-Ливень - 0.0
-Снег - 0.07</t>
+          <t>Дождь - 0.0
+Ливень - 0.0
+Снег - 0.0</t>
         </is>
       </c>
       <c r="F9" s="1" t="n">
-        <v>45580.69893958305</v>
+        <v>45580.99396962391</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>6.1</v>
+        <v>5.9</v>
       </c>
       <c r="B10" t="n">
-        <v>5.8</v>
+        <v>6</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Ю</t>
+          <t>ЮЗ</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>992.8</v>
+        <v>994.9</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Дождь - 0.4
+          <t>Дождь - 0.8
 Ливень - 0.0
 Снег - 0.07</t>
         </is>
       </c>
       <c r="F10" s="1" t="n">
-        <v>45580.69881643532</v>
+        <v>45580.99390919802</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>6.1</v>
+        <v>5.9</v>
       </c>
       <c r="B11" t="n">
-        <v>5.8</v>
+        <v>6</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Ю</t>
+          <t>ЮЗ</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>992.8</v>
+        <v>994.9</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Дождь - 0.4
+          <t>Дождь - 0.8
 Ливень - 0.0
 Снег - 0.07</t>
         </is>
       </c>
       <c r="F11" s="1" t="n">
-        <v>45580.6987004267</v>
+        <v>45580.99379513197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>